<commit_message>
Web Development Basics - HW 1 completed
</commit_message>
<xml_diff>
--- a/SoftUni-Level3/3.WebServices-and-Cloud/Web-Services-and-Cloud-Mar-2015-Schedule.xlsx
+++ b/SoftUni-Level3/3.WebServices-and-Cloud/Web-Services-and-Cloud-Mar-2015-Schedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
   <si>
     <t>Lecture</t>
   </si>
@@ -82,9 +82,6 @@
     <t>ASP.NET Web API</t>
   </si>
   <si>
-    <t>Web Services Unit Testing</t>
-  </si>
-  <si>
     <t>WCF</t>
   </si>
   <si>
@@ -134,6 +131,12 @@
   </si>
   <si>
     <t>Deployment of REST Services in Cloud</t>
+  </si>
+  <si>
+    <t>Teamwork Defense</t>
+  </si>
+  <si>
+    <t>Unit Testing Web Services</t>
   </si>
 </sst>
 </file>
@@ -227,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -314,6 +317,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -445,8 +451,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:G16" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:G17" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G17"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Number" dataDxfId="6"/>
     <tableColumn id="2" name="Lecture" dataDxfId="5"/>
@@ -747,15 +753,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="55" style="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="14" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" style="20" bestFit="1" customWidth="1"/>
@@ -815,7 +821,7 @@
         <v>20</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="15">
         <v>42093</v>
@@ -836,7 +842,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="22">
         <v>42095</v>
@@ -845,7 +851,7 @@
         <v>7</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="10"/>
     </row>
@@ -854,10 +860,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="D5" s="23">
         <v>42097</v>
@@ -875,10 +881,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" s="23">
         <v>42100</v>
@@ -886,31 +892,31 @@
       <c r="E6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="10"/>
+      <c r="F6" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="28"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="22">
+        <v>31</v>
+      </c>
+      <c r="D7" s="23">
         <v>42102</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="10"/>
+      <c r="F7" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="28"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
@@ -936,10 +942,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="23">
         <v>42108</v>
@@ -956,10 +962,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="23">
         <v>42109</v>
@@ -968,7 +974,7 @@
         <v>7</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G10" s="10"/>
     </row>
@@ -976,96 +982,115 @@
       <c r="A11" s="5">
         <v>9</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="30">
+        <v>42109</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="15"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="23">
+      <c r="C12" s="6"/>
+      <c r="D12" s="23">
         <v>42111</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E12" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F12" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="16"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="17">
         <v>11</v>
       </c>
-      <c r="D12" s="23">
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="23">
         <v>42113</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E13" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="F13" s="20" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="26"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="6" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="27"/>
+      <c r="D14" s="24"/>
       <c r="E14" s="25"/>
       <c r="F14" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="28"/>
+      <c r="G14" s="26"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15" t="s">
+      <c r="D15" s="27"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="26" t="s">
         <v>18</v>
       </c>
+      <c r="G15" s="28"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="6" t="s">
+      <c r="A16" s="17"/>
+      <c r="B16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="29"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="28" t="s">
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="28"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="29"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>